<commit_message>
Upload file error/success message
</commit_message>
<xml_diff>
--- a/Hyperbus/src/assets/Download Sample Format.xlsx
+++ b/Hyperbus/src/assets/Download Sample Format.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3BBBC1-8C51-4E97-A7F9-58ACC1588157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="13155" yWindow="4095" windowWidth="11790" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13158" yWindow="4098" windowWidth="11790" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>S.No</t>
   </si>
@@ -37,33 +31,6 @@
     <t>endDate</t>
   </si>
   <si>
-    <t>S2018056</t>
-  </si>
-  <si>
-    <t>Suma Shreya</t>
-  </si>
-  <si>
-    <t>T V</t>
-  </si>
-  <si>
-    <t>IIIT Sri City</t>
-  </si>
-  <si>
-    <t>B.Tech In CSE</t>
-  </si>
-  <si>
-    <t>S2019066</t>
-  </si>
-  <si>
-    <t>Shravani</t>
-  </si>
-  <si>
-    <t>Amity University</t>
-  </si>
-  <si>
-    <t>BCA</t>
-  </si>
-  <si>
     <t>middleName</t>
   </si>
   <si>
@@ -76,61 +43,13 @@
     <t>department</t>
   </si>
   <si>
-    <t>DUCS</t>
-  </si>
-  <si>
     <t>issuingAuthority</t>
-  </si>
-  <si>
-    <t>S2019076</t>
-  </si>
-  <si>
-    <t>S2019086</t>
-  </si>
-  <si>
-    <t>S2019096</t>
-  </si>
-  <si>
-    <t>Vaishnavi</t>
-  </si>
-  <si>
-    <t>Verma</t>
-  </si>
-  <si>
-    <t>DU</t>
-  </si>
-  <si>
-    <t>M.Sc</t>
-  </si>
-  <si>
-    <t>Niharika</t>
-  </si>
-  <si>
-    <t>GU</t>
-  </si>
-  <si>
-    <t>MBA</t>
-  </si>
-  <si>
-    <t>Khushi</t>
-  </si>
-  <si>
-    <t>Gupta</t>
-  </si>
-  <si>
-    <t>NIT</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Tech </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -284,7 +203,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -478,29 +397,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.68359375" customWidth="1"/>
+    <col min="3" max="4" width="18.26171875" customWidth="1"/>
+    <col min="5" max="5" width="20.26171875" customWidth="1"/>
+    <col min="6" max="7" width="20.41796875" customWidth="1"/>
+    <col min="8" max="8" width="19.68359375" customWidth="1"/>
+    <col min="9" max="9" width="13.578125" customWidth="1"/>
+    <col min="10" max="10" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -508,25 +427,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -536,149 +455,30 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="3">
-        <v>43325</v>
-      </c>
-      <c r="J2" s="3">
-        <v>44786</v>
-      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3">
-        <v>42960</v>
-      </c>
-      <c r="J3" s="3">
-        <v>43690</v>
-      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="3">
-        <v>44369</v>
-      </c>
-      <c r="J4" s="3">
-        <v>45099</v>
-      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="3">
-        <v>44734</v>
-      </c>
-      <c r="J5" s="3">
-        <v>45465</v>
-      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="3">
-        <v>43618</v>
-      </c>
-      <c r="J6" s="3">
-        <v>41427</v>
-      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed S.No from Sample file
</commit_message>
<xml_diff>
--- a/Hyperbus/src/assets/Download Sample Format.xlsx
+++ b/Hyperbus/src/assets/Download Sample Format.xlsx
@@ -4,20 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="13158" yWindow="4098" windowWidth="11790" windowHeight="11388"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23232" windowHeight="13152"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>S.No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>firstName</t>
   </si>
@@ -50,20 +47,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,11 +76,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,80 +392,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.68359375" customWidth="1"/>
-    <col min="3" max="4" width="18.26171875" customWidth="1"/>
-    <col min="5" max="5" width="20.26171875" customWidth="1"/>
-    <col min="6" max="7" width="20.41796875" customWidth="1"/>
-    <col min="8" max="8" width="19.68359375" customWidth="1"/>
-    <col min="9" max="9" width="13.578125" customWidth="1"/>
-    <col min="10" max="10" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.68359375" customWidth="1"/>
+    <col min="2" max="3" width="18.26171875" customWidth="1"/>
+    <col min="4" max="4" width="20.26171875" customWidth="1"/>
+    <col min="5" max="6" width="20.41796875" customWidth="1"/>
+    <col min="7" max="7" width="19.68359375" customWidth="1"/>
+    <col min="8" max="8" width="13.578125" customWidth="1"/>
+    <col min="9" max="9" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>